<commit_message>
Uploaded all changes before advancements and polishing
</commit_message>
<xml_diff>
--- a/static/top_10_habitable_exoplanets.xlsx
+++ b/static/top_10_habitable_exoplanets.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,16 +665,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9</v>
+        <v>1.1</v>
       </c>
       <c r="C7" t="n">
-        <v>2.8</v>
+        <v>1.05</v>
       </c>
       <c r="D7" t="n">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="E7" t="n">
         <v>10.35852619955</v>
@@ -697,18 +697,18 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>0.964816510677338</v>
+        <v>0.974672675132751</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>1.6</v>
+        <v>1.1</v>
       </c>
       <c r="C8" t="n">
-        <v>3.2</v>
+        <v>1.05</v>
       </c>
       <c r="D8" t="n">
         <v>300</v>
@@ -734,21 +734,21 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>0.951793611049652</v>
+        <v>0.974672675132751</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B9" t="n">
-        <v>3.8</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>1.1</v>
       </c>
       <c r="D9" t="n">
-        <v>550</v>
+        <v>300</v>
       </c>
       <c r="E9" t="n">
         <v>10.35852619955</v>
@@ -771,21 +771,21 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>5.19418881594902e-06</v>
+        <v>0.972165942192078</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>2.4</v>
+        <v>0.9</v>
       </c>
       <c r="C10" t="n">
-        <v>7.8</v>
+        <v>2.8</v>
       </c>
       <c r="D10" t="n">
-        <v>420</v>
+        <v>270</v>
       </c>
       <c r="E10" t="n">
         <v>10.35852619955</v>
@@ -808,7 +808,44 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>5.19418881594902e-06</v>
+        <v>0.964816510677338</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="D11" t="n">
+        <v>300</v>
+      </c>
+      <c r="E11" t="n">
+        <v>10.35852619955</v>
+      </c>
+      <c r="F11" t="n">
+        <v>531.944</v>
+      </c>
+      <c r="G11" t="n">
+        <v>5590.19</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.103</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>0.951793611049652</v>
       </c>
     </row>
   </sheetData>

</xml_diff>